<commit_message>
entry duplicate in data required
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>process</t>
   </si>
@@ -82,13 +82,46 @@
     <t>pe5</t>
   </si>
   <si>
-    <t>s1</t>
-  </si>
-  <si>
     <t>d6</t>
   </si>
   <si>
     <t>pe6</t>
+  </si>
+  <si>
+    <t>step_name</t>
+  </si>
+  <si>
+    <t>risk_name</t>
+  </si>
+  <si>
+    <t>wsp1</t>
+  </si>
+  <si>
+    <t>wsp2</t>
+  </si>
+  <si>
+    <t>wsp3</t>
+  </si>
+  <si>
+    <t>wsp4</t>
+  </si>
+  <si>
+    <t>wsp5</t>
+  </si>
+  <si>
+    <t>wsp6</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>r3</t>
+  </si>
+  <si>
+    <t>r4</t>
   </si>
 </sst>
 </file>
@@ -415,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,9 +460,11 @@
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,8 +477,14 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -456,8 +497,14 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -470,8 +517,14 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -484,8 +537,14 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -498,8 +557,14 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -512,19 +577,31 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel uploaded in database successfully
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>process</t>
   </si>
@@ -67,9 +67,6 @@
     <t>pe3</t>
   </si>
   <si>
-    <t>s2</t>
-  </si>
-  <si>
     <t>D4</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>pe5</t>
   </si>
   <si>
-    <t>d6</t>
-  </si>
-  <si>
     <t>pe6</t>
   </si>
   <si>
@@ -122,13 +116,82 @@
   </si>
   <si>
     <t>r4</t>
+  </si>
+  <si>
+    <t>sub_process</t>
+  </si>
+  <si>
+    <t>sp1</t>
+  </si>
+  <si>
+    <t>sp2</t>
+  </si>
+  <si>
+    <t>sp3</t>
+  </si>
+  <si>
+    <t>sp4</t>
+  </si>
+  <si>
+    <t>sp5</t>
+  </si>
+  <si>
+    <t>sp6</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>wsp7</t>
+  </si>
+  <si>
+    <t>r6</t>
+  </si>
+  <si>
+    <t>p2S1</t>
+  </si>
+  <si>
+    <t>p3S3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>P4S4</t>
+  </si>
+  <si>
+    <t>DP4</t>
+  </si>
+  <si>
+    <t>Pe7</t>
+  </si>
+  <si>
+    <t>wsps4</t>
+  </si>
+  <si>
+    <t>risk2</t>
+  </si>
+  <si>
+    <t>DP5</t>
+  </si>
+  <si>
+    <t>Pe8</t>
+  </si>
+  <si>
+    <t>wsps5</t>
+  </si>
+  <si>
+    <t>risk3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +203,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,14 +240,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -448,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,12 +540,12 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.85546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,13 +559,16 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -498,13 +582,16 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -518,13 +605,16 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -538,33 +628,39 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -572,36 +668,102 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>